<commit_message>
updated Sweden to 2020-04-05
</commit_message>
<xml_diff>
--- a/sweden/covid_deaths/Folkhalsomyndigheten_Covid19.xlsx
+++ b/sweden/covid_deaths/Folkhalsomyndigheten_Covid19.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19695" windowHeight="10455" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" firstSheet="4" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Antal per dag region" sheetId="1" r:id="rId1"/>
@@ -18,14 +18,14 @@
     <sheet name="Totalt antal per region" sheetId="4" r:id="rId4"/>
     <sheet name="Totalt antal per kön" sheetId="5" r:id="rId5"/>
     <sheet name="Totalt antal per åldersgrupp" sheetId="6" r:id="rId6"/>
-    <sheet name="FOHM 12 Apr 2020" sheetId="7" r:id="rId7"/>
+    <sheet name="FOHM 14 Apr 2020" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="50">
   <si>
     <t>Statistikdatum</t>
   </si>
@@ -175,9 +175,6 @@
   </si>
   <si>
     <t>Data uppdateras dagligen kl 11.30 och finns tillgägliga dagligen kl 14.00. Läs mer på https://www.folkhalsomyndigheten.se/smittskydd-beredskap/utbrott/aktuella-utbrott/covid-19/aktuellt-epidemiologiskt-lage/</t>
-  </si>
-  <si>
-    <t>uppgift saknas</t>
   </si>
 </sst>
 </file>
@@ -508,15 +505,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W70"/>
+  <dimension ref="A1:W72"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="13.140625" customWidth="1"/>
+    <col min="1" max="1" width="13.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23">
@@ -3577,7 +3574,7 @@
         <v>43907</v>
       </c>
       <c r="B44" s="2">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C44" s="2">
         <v>1</v>
@@ -3625,7 +3622,7 @@
         <v>1</v>
       </c>
       <c r="R44" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="S44" s="2">
         <v>1</v>
@@ -4358,7 +4355,7 @@
         <v>43918</v>
       </c>
       <c r="B55" s="2">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C55" s="2">
         <v>0</v>
@@ -4397,7 +4394,7 @@
         <v>147</v>
       </c>
       <c r="O55" s="2">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="P55" s="2">
         <v>7</v>
@@ -4500,7 +4497,7 @@
         <v>43920</v>
       </c>
       <c r="B57" s="2">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="C57" s="2">
         <v>0</v>
@@ -4536,7 +4533,7 @@
         <v>5</v>
       </c>
       <c r="N57" s="2">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="O57" s="2">
         <v>60</v>
@@ -5210,7 +5207,7 @@
         <v>43930</v>
       </c>
       <c r="B67" s="2">
-        <v>642</v>
+        <v>645</v>
       </c>
       <c r="C67" s="2">
         <v>1</v>
@@ -5267,10 +5264,10 @@
         <v>24</v>
       </c>
       <c r="U67" s="2">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="V67" s="2">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="W67" s="2">
         <v>54</v>
@@ -5281,7 +5278,7 @@
         <v>43931</v>
       </c>
       <c r="B68" s="2">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C68" s="2">
         <v>1</v>
@@ -5317,7 +5314,7 @@
         <v>24</v>
       </c>
       <c r="N68" s="2">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="O68" s="2">
         <v>41</v>
@@ -5352,13 +5349,13 @@
         <v>43932</v>
       </c>
       <c r="B69" s="2">
-        <v>330</v>
+        <v>390</v>
       </c>
       <c r="C69" s="2">
         <v>0</v>
       </c>
       <c r="D69" s="2">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E69" s="2">
         <v>0</v>
@@ -5373,7 +5370,7 @@
         <v>2</v>
       </c>
       <c r="I69" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="J69" s="2">
         <v>3</v>
@@ -5382,19 +5379,19 @@
         <v>10</v>
       </c>
       <c r="L69" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M69" s="2">
         <v>6</v>
       </c>
       <c r="N69" s="2">
-        <v>187</v>
+        <v>201</v>
       </c>
       <c r="O69" s="2">
         <v>22</v>
       </c>
       <c r="P69" s="2">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="Q69" s="2">
         <v>2</v>
@@ -5406,10 +5403,10 @@
         <v>0</v>
       </c>
       <c r="T69" s="2">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="U69" s="2">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="V69" s="2">
         <v>8</v>
@@ -5423,70 +5420,212 @@
         <v>43933</v>
       </c>
       <c r="B70" s="2">
-        <v>99</v>
+        <v>455</v>
       </c>
       <c r="C70" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D70" s="2">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="E70" s="2">
         <v>0</v>
       </c>
       <c r="F70" s="2">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="G70" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H70" s="2">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="I70" s="2">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="J70" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K70" s="2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L70" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="M70" s="2">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="N70" s="2">
-        <v>83</v>
+        <v>182</v>
       </c>
       <c r="O70" s="2">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="P70" s="2">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="Q70" s="2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="R70" s="2">
         <v>0</v>
       </c>
       <c r="S70" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="T70" s="2">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="U70" s="2">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="V70" s="2">
-        <v>0</v>
+        <v>64</v>
       </c>
       <c r="W70" s="2">
-        <v>0</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="71" spans="1:23">
+      <c r="A71" s="1">
+        <v>43934</v>
+      </c>
+      <c r="B71" s="2">
+        <v>421</v>
+      </c>
+      <c r="C71" s="2">
+        <v>0</v>
+      </c>
+      <c r="D71" s="2">
+        <v>12</v>
+      </c>
+      <c r="E71" s="2">
+        <v>0</v>
+      </c>
+      <c r="F71" s="2">
+        <v>11</v>
+      </c>
+      <c r="G71" s="2">
+        <v>3</v>
+      </c>
+      <c r="H71" s="2">
+        <v>6</v>
+      </c>
+      <c r="I71" s="2">
+        <v>5</v>
+      </c>
+      <c r="J71" s="2">
+        <v>6</v>
+      </c>
+      <c r="K71" s="2">
+        <v>3</v>
+      </c>
+      <c r="L71" s="2">
+        <v>17</v>
+      </c>
+      <c r="M71" s="2">
+        <v>9</v>
+      </c>
+      <c r="N71" s="2">
+        <v>201</v>
+      </c>
+      <c r="O71" s="2">
+        <v>20</v>
+      </c>
+      <c r="P71" s="2">
+        <v>13</v>
+      </c>
+      <c r="Q71" s="2">
+        <v>3</v>
+      </c>
+      <c r="R71" s="2">
+        <v>5</v>
+      </c>
+      <c r="S71" s="2">
+        <v>6</v>
+      </c>
+      <c r="T71" s="2">
+        <v>18</v>
+      </c>
+      <c r="U71" s="2">
+        <v>48</v>
+      </c>
+      <c r="V71" s="2">
+        <v>4</v>
+      </c>
+      <c r="W71" s="2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="72" spans="1:23">
+      <c r="A72" s="1">
+        <v>43935</v>
+      </c>
+      <c r="B72" s="2">
+        <v>124</v>
+      </c>
+      <c r="C72" s="2">
+        <v>0</v>
+      </c>
+      <c r="D72" s="2">
+        <v>0</v>
+      </c>
+      <c r="E72" s="2">
+        <v>0</v>
+      </c>
+      <c r="F72" s="2">
+        <v>0</v>
+      </c>
+      <c r="G72" s="2">
+        <v>1</v>
+      </c>
+      <c r="H72" s="2">
+        <v>0</v>
+      </c>
+      <c r="I72" s="2">
+        <v>0</v>
+      </c>
+      <c r="J72" s="2">
+        <v>3</v>
+      </c>
+      <c r="K72" s="2">
+        <v>0</v>
+      </c>
+      <c r="L72" s="2">
+        <v>3</v>
+      </c>
+      <c r="M72" s="2">
+        <v>0</v>
+      </c>
+      <c r="N72" s="2">
+        <v>95</v>
+      </c>
+      <c r="O72" s="2">
+        <v>0</v>
+      </c>
+      <c r="P72" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q72" s="2">
+        <v>0</v>
+      </c>
+      <c r="R72" s="2">
+        <v>0</v>
+      </c>
+      <c r="S72" s="2">
+        <v>0</v>
+      </c>
+      <c r="T72" s="2">
+        <v>11</v>
+      </c>
+      <c r="U72" s="2">
+        <v>4</v>
+      </c>
+      <c r="V72" s="2">
+        <v>0</v>
+      </c>
+      <c r="W72" s="2">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -5496,15 +5635,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B35"/>
+  <dimension ref="A1:B37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" customWidth="1"/>
+    <col min="1" max="1" width="12.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -5568,7 +5707,7 @@
         <v>43907</v>
       </c>
       <c r="B8" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -5656,7 +5795,7 @@
         <v>43918</v>
       </c>
       <c r="B19" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -5664,7 +5803,7 @@
         <v>43919</v>
       </c>
       <c r="B20" s="2">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -5672,7 +5811,7 @@
         <v>43920</v>
       </c>
       <c r="B21" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -5680,7 +5819,7 @@
         <v>43921</v>
       </c>
       <c r="B22" s="2">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -5688,7 +5827,7 @@
         <v>43922</v>
       </c>
       <c r="B23" s="2">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -5696,7 +5835,7 @@
         <v>43923</v>
       </c>
       <c r="B24" s="2">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -5704,7 +5843,7 @@
         <v>43924</v>
       </c>
       <c r="B25" s="2">
-        <v>65</v>
+        <v>68</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -5712,7 +5851,7 @@
         <v>43925</v>
       </c>
       <c r="B26" s="2">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -5720,7 +5859,7 @@
         <v>43926</v>
       </c>
       <c r="B27" s="2">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -5728,7 +5867,7 @@
         <v>43927</v>
       </c>
       <c r="B28" s="2">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -5736,7 +5875,7 @@
         <v>43928</v>
       </c>
       <c r="B29" s="2">
-        <v>60</v>
+        <v>65</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -5744,7 +5883,7 @@
         <v>43929</v>
       </c>
       <c r="B30" s="2">
-        <v>70</v>
+        <v>77</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -5752,7 +5891,7 @@
         <v>43930</v>
       </c>
       <c r="B31" s="2">
-        <v>24</v>
+        <v>43</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -5760,7 +5899,7 @@
         <v>43931</v>
       </c>
       <c r="B32" s="2">
-        <v>14</v>
+        <v>31</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -5768,7 +5907,7 @@
         <v>43932</v>
       </c>
       <c r="B33" s="2">
-        <v>8</v>
+        <v>26</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -5776,15 +5915,31 @@
         <v>43933</v>
       </c>
       <c r="B34" s="2">
-        <v>2</v>
+        <v>33</v>
       </c>
     </row>
     <row r="35" spans="1:2">
-      <c r="A35" s="1" t="s">
-        <v>50</v>
+      <c r="A35" s="1">
+        <v>43934</v>
       </c>
       <c r="B35" s="2">
-        <v>13</v>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="1">
+        <v>43935</v>
+      </c>
+      <c r="B36" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B37" s="2">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -5794,13 +5949,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B39"/>
+  <dimension ref="A1:B41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+    <sheetView topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="B33" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="15.36328125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -5975,7 +6133,7 @@
         <v>43916</v>
       </c>
       <c r="B22" s="2">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -6031,7 +6189,7 @@
         <v>43923</v>
       </c>
       <c r="B29" s="2">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -6055,7 +6213,7 @@
         <v>43926</v>
       </c>
       <c r="B32" s="2">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -6063,7 +6221,7 @@
         <v>43927</v>
       </c>
       <c r="B33" s="2">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -6071,7 +6229,7 @@
         <v>43928</v>
       </c>
       <c r="B34" s="2">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -6087,7 +6245,7 @@
         <v>43930</v>
       </c>
       <c r="B36" s="2">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -6095,7 +6253,7 @@
         <v>43931</v>
       </c>
       <c r="B37" s="2">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -6103,7 +6261,7 @@
         <v>43932</v>
       </c>
       <c r="B38" s="2">
-        <v>36</v>
+        <v>41</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -6111,7 +6269,23 @@
         <v>43933</v>
       </c>
       <c r="B39" s="2">
-        <v>1</v>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" s="1">
+        <v>43934</v>
+      </c>
+      <c r="B40" s="2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" s="1">
+        <v>43935</v>
+      </c>
+      <c r="B41" s="2">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -6127,7 +6301,7 @@
       <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
@@ -6151,16 +6325,16 @@
         <v>2</v>
       </c>
       <c r="B2" s="2">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C2" s="2">
-        <v>25.688257217407227</v>
+        <v>26.314800262451172</v>
       </c>
       <c r="D2" s="2">
         <v>3</v>
       </c>
       <c r="E2" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -6168,16 +6342,16 @@
         <v>3</v>
       </c>
       <c r="B3" s="2">
-        <v>316</v>
+        <v>365</v>
       </c>
       <c r="C3" s="2">
-        <v>109.73517608642578</v>
+        <v>126.75107574462891</v>
       </c>
       <c r="D3" s="2">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="E3" s="2">
-        <v>37</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -6191,7 +6365,7 @@
         <v>26.806957244873047</v>
       </c>
       <c r="D4" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E4" s="2">
         <v>0</v>
@@ -6202,16 +6376,16 @@
         <v>5</v>
       </c>
       <c r="B5" s="2">
-        <v>273</v>
+        <v>301</v>
       </c>
       <c r="C5" s="2">
-        <v>94.995513916015625</v>
+        <v>104.73863983154297</v>
       </c>
       <c r="D5" s="2">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E5" s="2">
-        <v>27</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -6219,16 +6393,16 @@
         <v>6</v>
       </c>
       <c r="B6" s="2">
-        <v>182</v>
+        <v>189</v>
       </c>
       <c r="C6" s="2">
-        <v>54.515827178955078</v>
+        <v>56.612590789794922</v>
       </c>
       <c r="D6" s="2">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E6" s="2">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -6236,10 +6410,10 @@
         <v>28</v>
       </c>
       <c r="B7" s="2">
-        <v>127</v>
+        <v>137</v>
       </c>
       <c r="C7" s="2">
-        <v>97.087379455566406</v>
+        <v>104.7320556640625</v>
       </c>
       <c r="D7" s="2">
         <v>4</v>
@@ -6253,16 +6427,16 @@
         <v>8</v>
       </c>
       <c r="B8" s="2">
-        <v>340</v>
+        <v>355</v>
       </c>
       <c r="C8" s="2">
-        <v>93.509605407714844</v>
+        <v>97.635032653808594</v>
       </c>
       <c r="D8" s="2">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E8" s="2">
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -6270,16 +6444,16 @@
         <v>9</v>
       </c>
       <c r="B9" s="2">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="C9" s="2">
-        <v>27.704668045043945</v>
+        <v>32.186305999755859</v>
       </c>
       <c r="D9" s="2">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E9" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -6287,13 +6461,13 @@
         <v>10</v>
       </c>
       <c r="B10" s="2">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="C10" s="2">
-        <v>48.146366119384766</v>
+        <v>51.620845794677734</v>
       </c>
       <c r="D10" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E10" s="2">
         <v>1</v>
@@ -6304,16 +6478,16 @@
         <v>11</v>
       </c>
       <c r="B11" s="2">
-        <v>134</v>
+        <v>157</v>
       </c>
       <c r="C11" s="2">
-        <v>53.580066680908203</v>
+        <v>62.776645660400391</v>
       </c>
       <c r="D11" s="2">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E11" s="2">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -6321,16 +6495,16 @@
         <v>12</v>
       </c>
       <c r="B12" s="2">
-        <v>435</v>
+        <v>458</v>
       </c>
       <c r="C12" s="2">
-        <v>31.571453094482422</v>
+        <v>33.240749359130859</v>
       </c>
       <c r="D12" s="2">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E12" s="2">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -6338,16 +6512,16 @@
         <v>13</v>
       </c>
       <c r="B13" s="2">
-        <v>4397</v>
+        <v>4806</v>
       </c>
       <c r="C13" s="2">
-        <v>184.97476196289063</v>
+        <v>202.18074035644531</v>
       </c>
       <c r="D13" s="2">
-        <v>368</v>
+        <v>396</v>
       </c>
       <c r="E13" s="2">
-        <v>528</v>
+        <v>616</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -6355,16 +6529,16 @@
         <v>14</v>
       </c>
       <c r="B14" s="2">
-        <v>661</v>
+        <v>694</v>
       </c>
       <c r="C14" s="2">
-        <v>222.15499877929688</v>
+        <v>233.24595642089844</v>
       </c>
       <c r="D14" s="2">
         <v>64</v>
       </c>
       <c r="E14" s="2">
-        <v>83</v>
+        <v>91</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -6372,16 +6546,16 @@
         <v>15</v>
       </c>
       <c r="B15" s="2">
-        <v>449</v>
+        <v>478</v>
       </c>
       <c r="C15" s="2">
-        <v>117.01454162597656</v>
+        <v>124.57227325439453</v>
       </c>
       <c r="D15" s="2">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="E15" s="2">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -6389,13 +6563,13 @@
         <v>16</v>
       </c>
       <c r="B16" s="2">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="C16" s="2">
-        <v>26.556756973266602</v>
+        <v>29.03538703918457</v>
       </c>
       <c r="D16" s="2">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E16" s="2">
         <v>1</v>
@@ -6406,16 +6580,16 @@
         <v>17</v>
       </c>
       <c r="B17" s="2">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="C17" s="2">
-        <v>67.344772338867188</v>
+        <v>68.816795349121094</v>
       </c>
       <c r="D17" s="2">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E17" s="2">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -6423,16 +6597,16 @@
         <v>18</v>
       </c>
       <c r="B18" s="2">
-        <v>100</v>
+        <v>111</v>
       </c>
       <c r="C18" s="2">
-        <v>40.758598327636719</v>
+        <v>45.242046356201172</v>
       </c>
       <c r="D18" s="2">
         <v>11</v>
       </c>
       <c r="E18" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -6440,16 +6614,16 @@
         <v>19</v>
       </c>
       <c r="B19" s="2">
-        <v>304</v>
+        <v>379</v>
       </c>
       <c r="C19" s="2">
-        <v>110.20681762695313</v>
+        <v>137.39599609375</v>
       </c>
       <c r="D19" s="2">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E19" s="2">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -6457,16 +6631,16 @@
         <v>29</v>
       </c>
       <c r="B20" s="2">
-        <v>1018</v>
+        <v>1106</v>
       </c>
       <c r="C20" s="2">
-        <v>58.984367370605469</v>
+        <v>64.083213806152344</v>
       </c>
       <c r="D20" s="2">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="E20" s="2">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -6474,16 +6648,16 @@
         <v>21</v>
       </c>
       <c r="B21" s="2">
-        <v>316</v>
+        <v>388</v>
       </c>
       <c r="C21" s="2">
-        <v>103.67283630371094</v>
+        <v>127.29450225830078</v>
       </c>
       <c r="D21" s="2">
         <v>26</v>
       </c>
       <c r="E21" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -6491,16 +6665,16 @@
         <v>22</v>
       </c>
       <c r="B22" s="2">
-        <v>951</v>
+        <v>1011</v>
       </c>
       <c r="C22" s="2">
-        <v>204.29864501953125</v>
+        <v>217.18815612792969</v>
       </c>
       <c r="D22" s="2">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E22" s="2">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -6513,10 +6687,10 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
@@ -6537,13 +6711,13 @@
         <v>34</v>
       </c>
       <c r="B2" s="2">
-        <v>5131</v>
+        <v>5586</v>
       </c>
       <c r="C2" s="2">
-        <v>633</v>
+        <v>688</v>
       </c>
       <c r="D2" s="2">
-        <v>523</v>
+        <v>594</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -6551,13 +6725,13 @@
         <v>35</v>
       </c>
       <c r="B3" s="2">
-        <v>5350</v>
+        <v>5857</v>
       </c>
       <c r="C3" s="2">
-        <v>206</v>
+        <v>227</v>
       </c>
       <c r="D3" s="2">
-        <v>376</v>
+        <v>439</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -6583,9 +6757,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
@@ -6606,10 +6782,10 @@
         <v>38</v>
       </c>
       <c r="B2" s="2">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C2" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D2" s="2">
         <v>0</v>
@@ -6620,7 +6796,7 @@
         <v>39</v>
       </c>
       <c r="B3" s="2">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="C3" s="2">
         <v>0</v>
@@ -6634,10 +6810,10 @@
         <v>40</v>
       </c>
       <c r="B4" s="2">
-        <v>767</v>
+        <v>833</v>
       </c>
       <c r="C4" s="2">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D4" s="2">
         <v>3</v>
@@ -6648,10 +6824,10 @@
         <v>41</v>
       </c>
       <c r="B5" s="2">
-        <v>978</v>
+        <v>1057</v>
       </c>
       <c r="C5" s="2">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="D5" s="2">
         <v>2</v>
@@ -6662,13 +6838,13 @@
         <v>42</v>
       </c>
       <c r="B6" s="2">
-        <v>1342</v>
+        <v>1460</v>
       </c>
       <c r="C6" s="2">
-        <v>97</v>
+        <v>113</v>
       </c>
       <c r="D6" s="2">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -6676,13 +6852,13 @@
         <v>43</v>
       </c>
       <c r="B7" s="2">
-        <v>1813</v>
+        <v>1961</v>
       </c>
       <c r="C7" s="2">
-        <v>210</v>
+        <v>223</v>
       </c>
       <c r="D7" s="2">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -6690,13 +6866,13 @@
         <v>44</v>
       </c>
       <c r="B8" s="2">
-        <v>1460</v>
+        <v>1590</v>
       </c>
       <c r="C8" s="2">
-        <v>255</v>
+        <v>279</v>
       </c>
       <c r="D8" s="2">
-        <v>64</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -6704,13 +6880,13 @@
         <v>45</v>
       </c>
       <c r="B9" s="2">
-        <v>1475</v>
+        <v>1617</v>
       </c>
       <c r="C9" s="2">
-        <v>173</v>
+        <v>188</v>
       </c>
       <c r="D9" s="2">
-        <v>231</v>
+        <v>256</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -6718,13 +6894,13 @@
         <v>46</v>
       </c>
       <c r="B10" s="2">
-        <v>1599</v>
+        <v>1778</v>
       </c>
       <c r="C10" s="2">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D10" s="2">
-        <v>366</v>
+        <v>430</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -6732,13 +6908,13 @@
         <v>47</v>
       </c>
       <c r="B11" s="2">
-        <v>819</v>
+        <v>916</v>
       </c>
       <c r="C11" s="2">
         <v>1</v>
       </c>
       <c r="D11" s="2">
-        <v>195</v>
+        <v>223</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -6746,7 +6922,7 @@
         <v>36</v>
       </c>
       <c r="B12" s="2">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C12" s="2">
         <v>0</v>
@@ -6764,9 +6940,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">

</xml_diff>